<commit_message>
added recovered dates to CP05MOAS
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00002.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="645" windowWidth="23205" windowHeight="8220" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="640" windowWidth="23200" windowHeight="8220" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -35,7 +30,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$99</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$386</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -404,9 +399,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,6 +453,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -609,7 +604,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -644,7 +639,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -855,60 +850,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="11" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="11" width="9.6640625" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:14" ht="28">
+      <c r="A1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="15">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -918,45 +913,47 @@
       <c r="C2" s="5">
         <v>335</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="19">
         <v>2</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="18">
         <v>42289</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>6.25E-2</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="22" t="s">
+      <c r="G2" s="28">
+        <v>42318</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="23">
+      <c r="J2" s="22">
         <v>200</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="24">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
         <v>39.833333333333336</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="24">
         <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
         <v>-70.708333333333329</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
@@ -975,563 +972,563 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:19" ht="28">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:19">
+      <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>335</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>643111</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="15">
         <v>0.61</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>335</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <v>643111</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>0.61</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>335</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>643111</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>0.61</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>335</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <v>643111</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <v>0.61</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-    </row>
-    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+    </row>
+    <row r="7" spans="1:19" s="2" customFormat="1">
+      <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>335</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>2</v>
       </c>
       <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="20">
         <v>2809</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="17">
         <v>117</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" s="2" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>335</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>2809</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>700</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" s="2" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>335</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>2</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="20">
         <v>2809</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>1.0760000000000001</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" s="2" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>335</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="20">
         <v>2809</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>3.9E-2</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:19" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" s="2" customFormat="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" s="2" customFormat="1">
+      <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>335</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <v>9029</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="9" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" s="2" customFormat="1">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" s="2" customFormat="1">
+      <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>335</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>2</v>
       </c>
       <c r="E14" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>105</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="9" t="s">
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" spans="1:19" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" s="2" customFormat="1">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" s="2" customFormat="1">
+      <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>335</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>2</v>
       </c>
       <c r="E16" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>50151</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="9">
         <v>1</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" s="2" customFormat="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" s="2" customFormat="1">
+      <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>335</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>2</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10">
         <v>335</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="9" t="s">
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" s="2" customFormat="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Pioneer gliders - fixed deployment dates
Fixed deployment dates based on cruise reports and WHOI documentation
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="640" windowWidth="23960" windowHeight="11220" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="12500" yWindow="2260" windowWidth="23960" windowHeight="11220" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -923,13 +923,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="18">
-        <v>42289</v>
+        <v>42291</v>
       </c>
       <c r="F2" s="6">
-        <v>6.25E-2</v>
+        <v>5.0694444444444452E-2</v>
       </c>
       <c r="G2" s="28">
-        <v>42318</v>
+        <v>42324</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>28</v>
@@ -978,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>